<commit_message>
updated test case template
</commit_message>
<xml_diff>
--- a/docs/contributions/AthanasiaZ/Writing-Charts/Phase6/TestCaseTemplate.xlsx
+++ b/docs/contributions/AthanasiaZ/Writing-Charts/Phase6/TestCaseTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\git-ΤΛ\nomnomr\docs\contributions\AthanasiaZ\Writing-Charts\Phase6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DC07DB-710E-4C72-8B24-21DE19EDC024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87EDBD62-AD06-4759-8A16-1C00171410D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BD39C543-FF37-421A-AB32-13E77B01613F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>TC_Order_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Π.χ. TC_NewAddress_01 </t>
   </si>
   <si>
     <t>Τι περιμένουμε να δούμε 
@@ -151,6 +148,16 @@
   <si>
     <t xml:space="preserve">Προφανώς η αρίθμηση των Test 
 Cases ξεκινάει ανά TC, αν υπάρχουν  4 TC_NewAddress θα έχουμε από  το 01 έως το 04, αν υπάρχουν 8  TC_TeamChoiceCategory θα έχουμε από το 01 έως το 08 κ.ο.κ.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Π.χ. 
+TC_NewAddress_01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Στην περίπτωση της 
+επιτυχημένης εισαγωγής 
+διεύθυνσης η ροή είναι Θετική.
+</t>
   </si>
 </sst>
 </file>
@@ -533,7 +540,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -571,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -579,7 +586,7 @@
     </row>
     <row r="2" spans="1:9" ht="138.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
@@ -588,25 +595,28 @@
         <v>9</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="4" t="s">
+        <v>30</v>
+      </c>
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
@@ -614,7 +624,7 @@
         <v>23</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -625,15 +635,15 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -641,7 +651,7 @@
         <v>14</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -649,12 +659,12 @@
         <v>15</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="103.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" s="3"/>
     </row>

</xml_diff>